<commit_message>
I think I only changed the path in the scrip_t4running_Associator_M
</commit_message>
<xml_diff>
--- a/RESULTS/RESULTS_Associator.xlsx
+++ b/RESULTS/RESULTS_Associator.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anna\SkyDrive\Documents\MATLAB\Associator_Mastersonvocab\RESULTS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="17610" windowHeight="7875"/>
+    <workbookView xWindow="483" yWindow="136" windowWidth="17612" windowHeight="7879"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="7" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -181,12 +176,15 @@
   </si>
   <si>
     <t>2016-02-05-21-42-46</t>
+  </si>
+  <si>
+    <t>2016-03-08-18-55-23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -354,7 +352,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -389,7 +387,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -602,25 +600,25 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F145" sqref="F145"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:AR3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="3" customWidth="1"/>
-    <col min="2" max="7" width="9.140625" style="3"/>
+    <col min="1" max="1" width="21.59765625" style="3" customWidth="1"/>
+    <col min="2" max="7" width="9.1328125" style="3"/>
     <col min="8" max="8" width="8" style="3" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" style="3" customWidth="1"/>
-    <col min="10" max="18" width="9.140625" style="3"/>
-    <col min="19" max="20" width="9.140625" style="13"/>
-    <col min="21" max="24" width="9.140625" style="3"/>
-    <col min="25" max="26" width="9.140625" style="2"/>
-    <col min="27" max="27" width="9.7109375" style="2" customWidth="1"/>
-    <col min="28" max="30" width="9.140625" style="2"/>
-    <col min="31" max="16384" width="9.140625" style="3"/>
+    <col min="9" max="9" width="8.59765625" style="3" customWidth="1"/>
+    <col min="10" max="18" width="9.1328125" style="3"/>
+    <col min="19" max="20" width="9.1328125" style="13"/>
+    <col min="21" max="24" width="9.1328125" style="3"/>
+    <col min="25" max="26" width="9.1328125" style="2"/>
+    <col min="27" max="27" width="9.73046875" style="2" customWidth="1"/>
+    <col min="28" max="30" width="9.1328125" style="2"/>
+    <col min="31" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" s="1" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" s="1" customFormat="1" ht="109.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -758,7 +756,7 @@
       </c>
       <c r="AX1" s="14"/>
     </row>
-    <row r="2" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>53</v>
       </c>
@@ -892,2177 +890,2307 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-    </row>
-    <row r="4" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="2">
+        <v>315</v>
+      </c>
+      <c r="C3" s="2">
+        <v>396</v>
+      </c>
+      <c r="D3" s="2">
+        <v>396</v>
+      </c>
+      <c r="E3" s="2">
+        <v>279</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4000</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1000</v>
+      </c>
+      <c r="K3" s="2">
+        <v>85.094093839999999</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1740</v>
+      </c>
+      <c r="O3" s="2">
+        <v>397</v>
+      </c>
+      <c r="P3" s="2">
+        <v>397</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>100</v>
+      </c>
+      <c r="R3" s="5">
+        <v>100</v>
+      </c>
+      <c r="S3" s="2">
+        <v>100</v>
+      </c>
+      <c r="T3" s="2">
+        <v>100</v>
+      </c>
+      <c r="U3" s="2">
+        <v>1</v>
+      </c>
+      <c r="V3" s="2">
+        <v>1</v>
+      </c>
+      <c r="W3" s="2">
+        <v>1</v>
+      </c>
+      <c r="X3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>100</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AO3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR3" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
     </row>
-    <row r="5" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
     </row>
-    <row r="6" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
     </row>
-    <row r="7" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
     </row>
-    <row r="8" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
     </row>
-    <row r="9" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
     </row>
-    <row r="10" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
     </row>
-    <row r="11" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
     </row>
-    <row r="12" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
     </row>
-    <row r="13" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
     </row>
-    <row r="14" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
     </row>
-    <row r="15" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
     </row>
-    <row r="16" spans="1:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:50" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
     </row>
-    <row r="17" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
     </row>
-    <row r="18" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
     </row>
-    <row r="19" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
     </row>
-    <row r="20" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
     </row>
-    <row r="21" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S21" s="5"/>
       <c r="T21" s="5"/>
     </row>
-    <row r="22" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
     </row>
-    <row r="23" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
     </row>
-    <row r="24" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S24" s="5"/>
       <c r="T24" s="5"/>
     </row>
-    <row r="25" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
     </row>
-    <row r="26" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
     </row>
-    <row r="27" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
     </row>
-    <row r="28" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S28" s="5"/>
       <c r="T28" s="5"/>
     </row>
-    <row r="29" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S29" s="5"/>
       <c r="T29" s="5"/>
     </row>
-    <row r="30" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S30" s="5"/>
       <c r="T30" s="5"/>
     </row>
-    <row r="31" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S31" s="5"/>
       <c r="T31" s="5"/>
     </row>
-    <row r="32" spans="9:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="9:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="I32" s="12"/>
       <c r="S32" s="5"/>
       <c r="T32" s="5"/>
     </row>
-    <row r="33" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="19:20" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="S33" s="5"/>
       <c r="T33" s="5"/>
     </row>
-    <row r="34" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S34" s="5"/>
       <c r="T34" s="5"/>
     </row>
-    <row r="35" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S35" s="5"/>
       <c r="T35" s="5"/>
     </row>
-    <row r="36" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S36" s="5"/>
       <c r="T36" s="5"/>
     </row>
-    <row r="37" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S37" s="5"/>
       <c r="T37" s="5"/>
     </row>
-    <row r="38" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S38" s="5"/>
       <c r="T38" s="5"/>
     </row>
-    <row r="39" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S39" s="5"/>
       <c r="T39" s="5"/>
     </row>
-    <row r="40" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
     </row>
-    <row r="41" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S41" s="5"/>
       <c r="T41" s="5"/>
     </row>
-    <row r="42" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S42" s="5"/>
       <c r="T42" s="5"/>
     </row>
-    <row r="43" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S43" s="5"/>
       <c r="T43" s="5"/>
     </row>
-    <row r="44" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S44" s="5"/>
       <c r="T44" s="5"/>
     </row>
-    <row r="45" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S45" s="5"/>
       <c r="T45" s="5"/>
     </row>
-    <row r="46" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S46" s="5"/>
       <c r="T46" s="5"/>
     </row>
-    <row r="47" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S47" s="5"/>
       <c r="T47" s="5"/>
     </row>
-    <row r="48" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S48" s="5"/>
       <c r="T48" s="5"/>
     </row>
-    <row r="49" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S49" s="5"/>
       <c r="T49" s="5"/>
     </row>
-    <row r="50" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S50" s="5"/>
       <c r="T50" s="5"/>
     </row>
-    <row r="51" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S51" s="5"/>
       <c r="T51" s="5"/>
     </row>
-    <row r="52" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S52" s="5"/>
       <c r="T52" s="5"/>
     </row>
-    <row r="53" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S53" s="5"/>
       <c r="T53" s="5"/>
     </row>
-    <row r="54" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S54" s="5"/>
       <c r="T54" s="5"/>
     </row>
-    <row r="55" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S55" s="5"/>
       <c r="T55" s="5"/>
     </row>
-    <row r="56" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S56" s="5"/>
       <c r="T56" s="5"/>
     </row>
-    <row r="57" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S57" s="5"/>
       <c r="T57" s="5"/>
     </row>
-    <row r="58" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S58" s="5"/>
       <c r="T58" s="5"/>
     </row>
-    <row r="59" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S59" s="5"/>
       <c r="T59" s="5"/>
     </row>
-    <row r="60" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S60" s="5"/>
       <c r="T60" s="5"/>
     </row>
-    <row r="61" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S61" s="5"/>
       <c r="T61" s="5"/>
     </row>
-    <row r="62" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S62" s="5"/>
       <c r="T62" s="5"/>
     </row>
-    <row r="63" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S63" s="5"/>
       <c r="T63" s="5"/>
     </row>
-    <row r="64" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S64" s="5"/>
       <c r="T64" s="5"/>
     </row>
-    <row r="65" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S65" s="5"/>
       <c r="T65" s="5"/>
     </row>
-    <row r="66" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S66" s="5"/>
       <c r="T66" s="5"/>
     </row>
-    <row r="67" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S67" s="5"/>
       <c r="T67" s="5"/>
     </row>
-    <row r="68" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S68" s="5"/>
       <c r="T68" s="5"/>
     </row>
-    <row r="69" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S69" s="5"/>
       <c r="T69" s="5"/>
     </row>
-    <row r="70" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S70" s="5"/>
       <c r="T70" s="5"/>
     </row>
-    <row r="71" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S71" s="5"/>
       <c r="T71" s="5"/>
     </row>
-    <row r="72" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S72" s="5"/>
       <c r="T72" s="5"/>
     </row>
-    <row r="73" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S73" s="5"/>
       <c r="T73" s="5"/>
     </row>
-    <row r="74" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S74" s="5"/>
       <c r="T74" s="5"/>
     </row>
-    <row r="75" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S75" s="5"/>
       <c r="T75" s="5"/>
     </row>
-    <row r="76" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S76" s="5"/>
       <c r="T76" s="5"/>
     </row>
-    <row r="77" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S77" s="5"/>
       <c r="T77" s="5"/>
     </row>
-    <row r="78" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S78" s="5"/>
       <c r="T78" s="5"/>
     </row>
-    <row r="79" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S79" s="5"/>
       <c r="T79" s="5"/>
     </row>
-    <row r="80" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S80" s="5"/>
       <c r="T80" s="5"/>
     </row>
-    <row r="81" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S81" s="5"/>
       <c r="T81" s="5"/>
     </row>
-    <row r="82" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S82" s="5"/>
       <c r="T82" s="5"/>
     </row>
-    <row r="83" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S83" s="5"/>
       <c r="T83" s="5"/>
     </row>
-    <row r="84" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S84" s="5"/>
       <c r="T84" s="5"/>
     </row>
-    <row r="85" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S85" s="5"/>
       <c r="T85" s="5"/>
     </row>
-    <row r="86" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S86" s="5"/>
       <c r="T86" s="5"/>
     </row>
-    <row r="87" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S87" s="5"/>
       <c r="T87" s="5"/>
     </row>
-    <row r="88" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S88" s="5"/>
       <c r="T88" s="5"/>
     </row>
-    <row r="89" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S89" s="5"/>
       <c r="T89" s="5"/>
     </row>
-    <row r="90" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S90" s="5"/>
       <c r="T90" s="5"/>
     </row>
-    <row r="91" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S91" s="5"/>
       <c r="T91" s="5"/>
     </row>
-    <row r="92" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S92" s="5"/>
       <c r="T92" s="5"/>
     </row>
-    <row r="93" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S93" s="5"/>
       <c r="T93" s="5"/>
     </row>
-    <row r="94" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S94" s="5"/>
       <c r="T94" s="5"/>
     </row>
-    <row r="95" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S95" s="5"/>
       <c r="T95" s="5"/>
     </row>
-    <row r="96" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S96" s="5"/>
       <c r="T96" s="5"/>
     </row>
-    <row r="97" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S97" s="5"/>
       <c r="T97" s="5"/>
     </row>
-    <row r="98" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S98" s="5"/>
       <c r="T98" s="5"/>
     </row>
-    <row r="99" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S99" s="5"/>
       <c r="T99" s="5"/>
     </row>
-    <row r="100" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S100" s="5"/>
       <c r="T100" s="5"/>
     </row>
-    <row r="101" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S101" s="5"/>
       <c r="T101" s="5"/>
     </row>
-    <row r="102" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S102" s="5"/>
       <c r="T102" s="5"/>
     </row>
-    <row r="103" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S103" s="5"/>
       <c r="T103" s="5"/>
     </row>
-    <row r="104" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S104" s="5"/>
       <c r="T104" s="5"/>
     </row>
-    <row r="105" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S105" s="5"/>
       <c r="T105" s="5"/>
     </row>
-    <row r="106" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="107" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S107" s="5"/>
       <c r="T107" s="5"/>
     </row>
-    <row r="108" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S108" s="5"/>
       <c r="T108" s="5"/>
     </row>
-    <row r="109" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S109" s="5"/>
       <c r="T109" s="5"/>
     </row>
-    <row r="110" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S110" s="5"/>
       <c r="T110" s="5"/>
     </row>
-    <row r="111" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S111" s="5"/>
       <c r="T111" s="5"/>
     </row>
-    <row r="112" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S112" s="5"/>
       <c r="T112" s="5"/>
     </row>
-    <row r="113" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S113" s="5"/>
       <c r="T113" s="5"/>
     </row>
-    <row r="114" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S114" s="5"/>
       <c r="T114" s="5"/>
     </row>
-    <row r="115" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S115" s="5"/>
       <c r="T115" s="5"/>
     </row>
-    <row r="116" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S116" s="5"/>
       <c r="T116" s="5"/>
     </row>
-    <row r="117" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S117" s="5"/>
       <c r="T117" s="5"/>
     </row>
-    <row r="118" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S118" s="5"/>
       <c r="T118" s="5"/>
     </row>
-    <row r="119" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S119" s="5"/>
       <c r="T119" s="5"/>
     </row>
-    <row r="120" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S120" s="5"/>
       <c r="T120" s="5"/>
     </row>
-    <row r="121" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S121" s="5"/>
       <c r="T121" s="5"/>
     </row>
-    <row r="122" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S122" s="5"/>
       <c r="T122" s="5"/>
     </row>
-    <row r="123" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S123" s="5"/>
       <c r="T123" s="5"/>
     </row>
-    <row r="124" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S124" s="5"/>
       <c r="T124" s="5"/>
     </row>
-    <row r="125" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S125" s="5"/>
       <c r="T125" s="5"/>
     </row>
-    <row r="126" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S126" s="5"/>
       <c r="T126" s="5"/>
     </row>
-    <row r="127" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S127" s="5"/>
       <c r="T127" s="5"/>
     </row>
-    <row r="128" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S128" s="5"/>
       <c r="T128" s="5"/>
     </row>
-    <row r="129" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S129" s="5"/>
       <c r="T129" s="5"/>
     </row>
-    <row r="130" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S130" s="5"/>
       <c r="T130" s="5"/>
     </row>
-    <row r="131" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S131" s="5"/>
       <c r="T131" s="5"/>
     </row>
-    <row r="132" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S132" s="5"/>
       <c r="T132" s="5"/>
     </row>
-    <row r="133" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S133" s="5"/>
       <c r="T133" s="5"/>
     </row>
-    <row r="134" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S134" s="5"/>
       <c r="T134" s="5"/>
     </row>
-    <row r="135" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S135" s="5"/>
       <c r="T135" s="5"/>
     </row>
-    <row r="136" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S136" s="5"/>
       <c r="T136" s="5"/>
     </row>
-    <row r="137" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S137" s="5"/>
       <c r="T137" s="5"/>
     </row>
-    <row r="138" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S138" s="5"/>
       <c r="T138" s="5"/>
     </row>
-    <row r="139" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S139" s="5"/>
       <c r="T139" s="5"/>
     </row>
-    <row r="140" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S140" s="5"/>
       <c r="T140" s="5"/>
     </row>
-    <row r="141" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S141" s="5"/>
       <c r="T141" s="5"/>
     </row>
-    <row r="142" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S142" s="5"/>
       <c r="T142" s="5"/>
     </row>
-    <row r="143" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S143" s="5"/>
       <c r="T143" s="5"/>
     </row>
-    <row r="144" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S144" s="5"/>
       <c r="T144" s="5"/>
     </row>
-    <row r="145" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S145" s="5"/>
       <c r="T145" s="5"/>
     </row>
-    <row r="146" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S146" s="5"/>
       <c r="T146" s="5"/>
     </row>
-    <row r="147" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S147" s="5"/>
       <c r="T147" s="5"/>
     </row>
-    <row r="148" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S148" s="5"/>
       <c r="T148" s="5"/>
     </row>
-    <row r="149" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S149" s="5"/>
       <c r="T149" s="5"/>
     </row>
-    <row r="150" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S150" s="5"/>
       <c r="T150" s="5"/>
     </row>
-    <row r="151" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S151" s="5"/>
       <c r="T151" s="5"/>
     </row>
-    <row r="152" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S152" s="5"/>
       <c r="T152" s="5"/>
     </row>
-    <row r="153" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S153" s="5"/>
       <c r="T153" s="5"/>
     </row>
-    <row r="154" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S154" s="5"/>
       <c r="T154" s="5"/>
     </row>
-    <row r="155" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S155" s="5"/>
       <c r="T155" s="5"/>
     </row>
-    <row r="156" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S156" s="5"/>
       <c r="T156" s="5"/>
     </row>
-    <row r="157" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S157" s="5"/>
       <c r="T157" s="5"/>
     </row>
-    <row r="158" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S158" s="5"/>
       <c r="T158" s="5"/>
     </row>
-    <row r="159" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S159" s="5"/>
       <c r="T159" s="5"/>
     </row>
-    <row r="160" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S160" s="5"/>
       <c r="T160" s="5"/>
     </row>
-    <row r="161" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S161" s="5"/>
       <c r="T161" s="5"/>
     </row>
-    <row r="162" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S162" s="5"/>
       <c r="T162" s="5"/>
     </row>
-    <row r="163" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S163" s="5"/>
       <c r="T163" s="5"/>
     </row>
-    <row r="164" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S164" s="5"/>
       <c r="T164" s="5"/>
     </row>
-    <row r="165" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S165" s="5"/>
       <c r="T165" s="5"/>
     </row>
-    <row r="166" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S166" s="5"/>
       <c r="T166" s="5"/>
     </row>
-    <row r="167" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S167" s="5"/>
       <c r="T167" s="5"/>
     </row>
-    <row r="168" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S168" s="5"/>
       <c r="T168" s="5"/>
     </row>
-    <row r="169" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S169" s="5"/>
       <c r="T169" s="5"/>
     </row>
-    <row r="170" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S170" s="5"/>
       <c r="T170" s="5"/>
     </row>
-    <row r="171" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S171" s="5"/>
       <c r="T171" s="5"/>
     </row>
-    <row r="172" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S172" s="5"/>
       <c r="T172" s="5"/>
     </row>
-    <row r="173" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S173" s="5"/>
       <c r="T173" s="5"/>
     </row>
-    <row r="174" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S174" s="5"/>
       <c r="T174" s="5"/>
     </row>
-    <row r="175" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S175" s="5"/>
       <c r="T175" s="5"/>
     </row>
-    <row r="176" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S176" s="5"/>
       <c r="T176" s="5"/>
     </row>
-    <row r="177" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S177" s="5"/>
       <c r="T177" s="5"/>
     </row>
-    <row r="178" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S178" s="5"/>
       <c r="T178" s="5"/>
     </row>
-    <row r="179" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S179" s="5"/>
       <c r="T179" s="5"/>
     </row>
-    <row r="180" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S180" s="5"/>
       <c r="T180" s="5"/>
     </row>
-    <row r="181" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S181" s="5"/>
       <c r="T181" s="5"/>
     </row>
-    <row r="182" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S182" s="5"/>
       <c r="T182" s="5"/>
     </row>
-    <row r="183" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S183" s="5"/>
       <c r="T183" s="5"/>
     </row>
-    <row r="184" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S184" s="5"/>
       <c r="T184" s="5"/>
     </row>
-    <row r="185" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S185" s="5"/>
       <c r="T185" s="5"/>
     </row>
-    <row r="186" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S186" s="5"/>
       <c r="T186" s="5"/>
     </row>
-    <row r="187" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S187" s="5"/>
       <c r="T187" s="5"/>
     </row>
-    <row r="188" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S188" s="5"/>
       <c r="T188" s="5"/>
     </row>
-    <row r="189" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S189" s="5"/>
       <c r="T189" s="5"/>
     </row>
-    <row r="190" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S190" s="5"/>
       <c r="T190" s="5"/>
     </row>
-    <row r="191" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S191" s="5"/>
       <c r="T191" s="5"/>
     </row>
-    <row r="192" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S192" s="5"/>
       <c r="T192" s="5"/>
     </row>
-    <row r="193" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S193" s="5"/>
       <c r="T193" s="5"/>
     </row>
-    <row r="194" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S194" s="5"/>
       <c r="T194" s="5"/>
     </row>
-    <row r="195" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S195" s="5"/>
       <c r="T195" s="5"/>
     </row>
-    <row r="196" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S196" s="5"/>
       <c r="T196" s="5"/>
     </row>
-    <row r="197" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S197" s="5"/>
       <c r="T197" s="5"/>
     </row>
-    <row r="198" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S198" s="5"/>
       <c r="T198" s="5"/>
     </row>
-    <row r="199" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S199" s="5"/>
       <c r="T199" s="5"/>
     </row>
-    <row r="200" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S200" s="5"/>
       <c r="T200" s="5"/>
     </row>
-    <row r="201" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S201" s="5"/>
       <c r="T201" s="5"/>
     </row>
-    <row r="202" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S202" s="5"/>
       <c r="T202" s="5"/>
     </row>
-    <row r="203" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S203" s="5"/>
       <c r="T203" s="5"/>
     </row>
-    <row r="204" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S204" s="5"/>
       <c r="T204" s="5"/>
     </row>
-    <row r="205" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S205" s="5"/>
       <c r="T205" s="5"/>
     </row>
-    <row r="206" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S206" s="5"/>
       <c r="T206" s="5"/>
     </row>
-    <row r="207" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S207" s="5"/>
       <c r="T207" s="5"/>
     </row>
-    <row r="208" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S208" s="5"/>
       <c r="T208" s="5"/>
     </row>
-    <row r="209" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S209" s="5"/>
       <c r="T209" s="5"/>
     </row>
-    <row r="210" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S210" s="5"/>
       <c r="T210" s="5"/>
     </row>
-    <row r="211" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S211" s="5"/>
       <c r="T211" s="5"/>
     </row>
-    <row r="212" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S212" s="5"/>
       <c r="T212" s="5"/>
     </row>
-    <row r="213" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S213" s="5"/>
       <c r="T213" s="5"/>
     </row>
-    <row r="214" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S214" s="5"/>
       <c r="T214" s="5"/>
     </row>
-    <row r="215" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S215" s="5"/>
       <c r="T215" s="5"/>
     </row>
-    <row r="216" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S216" s="5"/>
       <c r="T216" s="5"/>
     </row>
-    <row r="217" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S217" s="5"/>
       <c r="T217" s="5"/>
     </row>
-    <row r="218" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S218" s="5"/>
       <c r="T218" s="5"/>
     </row>
-    <row r="219" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S219" s="5"/>
       <c r="T219" s="5"/>
     </row>
-    <row r="220" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S220" s="5"/>
       <c r="T220" s="5"/>
     </row>
-    <row r="221" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S221" s="5"/>
       <c r="T221" s="5"/>
     </row>
-    <row r="222" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S222" s="5"/>
       <c r="T222" s="5"/>
     </row>
-    <row r="223" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S223" s="5"/>
       <c r="T223" s="5"/>
     </row>
-    <row r="224" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="19:20" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S224" s="5"/>
       <c r="T224" s="5"/>
     </row>
-    <row r="225" spans="19:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="19:50" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S225" s="5"/>
       <c r="T225" s="5"/>
     </row>
-    <row r="226" spans="19:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="19:50" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S226" s="5"/>
       <c r="T226" s="5"/>
     </row>
-    <row r="227" spans="19:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="19:50" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S227" s="5"/>
       <c r="T227" s="5"/>
     </row>
-    <row r="228" spans="19:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="19:50" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S228" s="5"/>
       <c r="T228" s="5"/>
     </row>
-    <row r="229" spans="19:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="19:50" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S229" s="5"/>
       <c r="T229" s="5"/>
     </row>
-    <row r="230" spans="19:50" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="19:50" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="S230" s="5"/>
       <c r="T230" s="5"/>
     </row>
-    <row r="231" spans="19:50" x14ac:dyDescent="0.25">
+    <row r="231" spans="19:50" x14ac:dyDescent="0.45">
       <c r="AW231" s="4"/>
       <c r="AX231" s="4"/>
     </row>
-    <row r="232" spans="19:50" x14ac:dyDescent="0.25">
+    <row r="232" spans="19:50" x14ac:dyDescent="0.45">
       <c r="AW232" s="4"/>
       <c r="AX232" s="4"/>
     </row>
-    <row r="233" spans="19:50" x14ac:dyDescent="0.25">
+    <row r="233" spans="19:50" x14ac:dyDescent="0.45">
       <c r="AW233" s="4"/>
       <c r="AX233" s="4"/>
     </row>
-    <row r="234" spans="19:50" x14ac:dyDescent="0.25">
+    <row r="234" spans="19:50" x14ac:dyDescent="0.45">
       <c r="AW234" s="4"/>
       <c r="AX234" s="4"/>
     </row>
-    <row r="235" spans="19:50" x14ac:dyDescent="0.25">
+    <row r="235" spans="19:50" x14ac:dyDescent="0.45">
       <c r="AW235" s="4"/>
       <c r="AX235" s="4"/>
     </row>
-    <row r="236" spans="19:50" x14ac:dyDescent="0.25">
+    <row r="236" spans="19:50" x14ac:dyDescent="0.45">
       <c r="AW236" s="4"/>
       <c r="AX236" s="4"/>
     </row>
-    <row r="237" spans="19:50" x14ac:dyDescent="0.25">
+    <row r="237" spans="19:50" x14ac:dyDescent="0.45">
       <c r="AW237" s="4"/>
       <c r="AX237" s="4"/>
     </row>
-    <row r="238" spans="19:50" x14ac:dyDescent="0.25">
+    <row r="238" spans="19:50" x14ac:dyDescent="0.45">
       <c r="AW238" s="4"/>
       <c r="AX238" s="4"/>
     </row>
-    <row r="239" spans="19:50" x14ac:dyDescent="0.25">
+    <row r="239" spans="19:50" x14ac:dyDescent="0.45">
       <c r="AW239" s="4"/>
       <c r="AX239" s="4"/>
     </row>
-    <row r="240" spans="19:50" x14ac:dyDescent="0.25">
+    <row r="240" spans="19:50" x14ac:dyDescent="0.45">
       <c r="AW240" s="4"/>
       <c r="AX240" s="4"/>
     </row>
-    <row r="241" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="241" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW241" s="4"/>
       <c r="AX241" s="4"/>
     </row>
-    <row r="242" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="242" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW242" s="4"/>
       <c r="AX242" s="4"/>
     </row>
-    <row r="243" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="243" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW243" s="4"/>
       <c r="AX243" s="4"/>
     </row>
-    <row r="244" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="244" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW244" s="4"/>
       <c r="AX244" s="4"/>
     </row>
-    <row r="245" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="245" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW245" s="4"/>
       <c r="AX245" s="4"/>
     </row>
-    <row r="246" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="246" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW246" s="4"/>
       <c r="AX246" s="4"/>
     </row>
-    <row r="247" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="247" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW247" s="4"/>
       <c r="AX247" s="4"/>
     </row>
-    <row r="248" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="248" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW248" s="4"/>
       <c r="AX248" s="4"/>
     </row>
-    <row r="249" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="249" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW249" s="4"/>
       <c r="AX249" s="4"/>
     </row>
-    <row r="250" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="250" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW250" s="4"/>
       <c r="AX250" s="4"/>
     </row>
-    <row r="251" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="251" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW251" s="4"/>
       <c r="AX251" s="4"/>
     </row>
-    <row r="252" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="252" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW252" s="4"/>
       <c r="AX252" s="4"/>
     </row>
-    <row r="253" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="253" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW253" s="4"/>
       <c r="AX253" s="4"/>
     </row>
-    <row r="254" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="254" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW254" s="4"/>
       <c r="AX254" s="4"/>
     </row>
-    <row r="255" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="255" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW255" s="4"/>
       <c r="AX255" s="4"/>
     </row>
-    <row r="256" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="256" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW256" s="4"/>
       <c r="AX256" s="4"/>
     </row>
-    <row r="257" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="257" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW257" s="4"/>
       <c r="AX257" s="4"/>
     </row>
-    <row r="258" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="258" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW258" s="4"/>
       <c r="AX258" s="4"/>
     </row>
-    <row r="259" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="259" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW259" s="4"/>
       <c r="AX259" s="4"/>
     </row>
-    <row r="260" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="260" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW260" s="4"/>
       <c r="AX260" s="4"/>
     </row>
-    <row r="261" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="261" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW261" s="4"/>
       <c r="AX261" s="4"/>
     </row>
-    <row r="262" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="262" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW262" s="4"/>
       <c r="AX262" s="4"/>
     </row>
-    <row r="263" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="263" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW263" s="4"/>
       <c r="AX263" s="4"/>
     </row>
-    <row r="264" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="264" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW264" s="4"/>
       <c r="AX264" s="4"/>
     </row>
-    <row r="265" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="265" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW265" s="4"/>
       <c r="AX265" s="4"/>
     </row>
-    <row r="266" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="266" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW266" s="4"/>
       <c r="AX266" s="4"/>
     </row>
-    <row r="267" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="267" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW267" s="4"/>
       <c r="AX267" s="4"/>
     </row>
-    <row r="268" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="268" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW268" s="4"/>
       <c r="AX268" s="4"/>
     </row>
-    <row r="269" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="269" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW269" s="4"/>
       <c r="AX269" s="4"/>
     </row>
-    <row r="270" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="270" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW270" s="4"/>
       <c r="AX270" s="4"/>
     </row>
-    <row r="271" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="271" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW271" s="4"/>
       <c r="AX271" s="4"/>
     </row>
-    <row r="272" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="272" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW272" s="4"/>
       <c r="AX272" s="4"/>
     </row>
-    <row r="273" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="273" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW273" s="4"/>
       <c r="AX273" s="4"/>
     </row>
-    <row r="274" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="274" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW274" s="4"/>
       <c r="AX274" s="4"/>
     </row>
-    <row r="275" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="275" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW275" s="4"/>
       <c r="AX275" s="4"/>
     </row>
-    <row r="276" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="276" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW276" s="4"/>
       <c r="AX276" s="4"/>
     </row>
-    <row r="277" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="277" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW277" s="4"/>
       <c r="AX277" s="4"/>
     </row>
-    <row r="278" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="278" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW278" s="4"/>
       <c r="AX278" s="4"/>
     </row>
-    <row r="279" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="279" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW279" s="4"/>
       <c r="AX279" s="4"/>
     </row>
-    <row r="280" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="280" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW280" s="4"/>
       <c r="AX280" s="4"/>
     </row>
-    <row r="281" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="281" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW281" s="4"/>
       <c r="AX281" s="4"/>
     </row>
-    <row r="282" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="282" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW282" s="4"/>
       <c r="AX282" s="4"/>
     </row>
-    <row r="283" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="283" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW283" s="4"/>
       <c r="AX283" s="4"/>
     </row>
-    <row r="284" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="284" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW284" s="4"/>
       <c r="AX284" s="4"/>
     </row>
-    <row r="285" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="285" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW285" s="4"/>
       <c r="AX285" s="4"/>
     </row>
-    <row r="286" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="286" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW286" s="4"/>
       <c r="AX286" s="4"/>
     </row>
-    <row r="287" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="287" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW287" s="4"/>
       <c r="AX287" s="4"/>
     </row>
-    <row r="288" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="288" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW288" s="4"/>
       <c r="AX288" s="4"/>
     </row>
-    <row r="289" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="289" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW289" s="4"/>
       <c r="AX289" s="4"/>
     </row>
-    <row r="290" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="290" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW290" s="4"/>
       <c r="AX290" s="4"/>
     </row>
-    <row r="291" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="291" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW291" s="4"/>
       <c r="AX291" s="4"/>
     </row>
-    <row r="292" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="292" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW292" s="4"/>
       <c r="AX292" s="4"/>
     </row>
-    <row r="293" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="293" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW293" s="4"/>
       <c r="AX293" s="4"/>
     </row>
-    <row r="294" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="294" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW294" s="4"/>
       <c r="AX294" s="4"/>
     </row>
-    <row r="295" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="295" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW295" s="4"/>
       <c r="AX295" s="4"/>
     </row>
-    <row r="296" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="296" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW296" s="4"/>
       <c r="AX296" s="4"/>
     </row>
-    <row r="297" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="297" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW297" s="4"/>
       <c r="AX297" s="4"/>
     </row>
-    <row r="298" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="298" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW298" s="4"/>
       <c r="AX298" s="4"/>
     </row>
-    <row r="299" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="299" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW299" s="4"/>
       <c r="AX299" s="4"/>
     </row>
-    <row r="300" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="300" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW300" s="4"/>
       <c r="AX300" s="4"/>
     </row>
-    <row r="301" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="301" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW301" s="4"/>
       <c r="AX301" s="4"/>
     </row>
-    <row r="302" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="302" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW302" s="4"/>
       <c r="AX302" s="4"/>
     </row>
-    <row r="303" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="303" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW303" s="4"/>
       <c r="AX303" s="4"/>
     </row>
-    <row r="304" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="304" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW304" s="4"/>
       <c r="AX304" s="4"/>
     </row>
-    <row r="305" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="305" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW305" s="4"/>
       <c r="AX305" s="4"/>
     </row>
-    <row r="306" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="306" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW306" s="4"/>
       <c r="AX306" s="4"/>
     </row>
-    <row r="307" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="307" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW307" s="4"/>
       <c r="AX307" s="4"/>
     </row>
-    <row r="308" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="308" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW308" s="4"/>
       <c r="AX308" s="4"/>
     </row>
-    <row r="309" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="309" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW309" s="4"/>
       <c r="AX309" s="4"/>
     </row>
-    <row r="310" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="310" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW310" s="4"/>
       <c r="AX310" s="4"/>
     </row>
-    <row r="311" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="311" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW311" s="4"/>
       <c r="AX311" s="4"/>
     </row>
-    <row r="312" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="312" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW312" s="4"/>
       <c r="AX312" s="4"/>
     </row>
-    <row r="313" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="313" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW313" s="4"/>
       <c r="AX313" s="4"/>
     </row>
-    <row r="314" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="314" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW314" s="4"/>
       <c r="AX314" s="4"/>
     </row>
-    <row r="315" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="315" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW315" s="4"/>
       <c r="AX315" s="4"/>
     </row>
-    <row r="316" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="316" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW316" s="4"/>
       <c r="AX316" s="4"/>
     </row>
-    <row r="317" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="317" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW317" s="4"/>
       <c r="AX317" s="4"/>
     </row>
-    <row r="318" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="318" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW318" s="4"/>
       <c r="AX318" s="4"/>
     </row>
-    <row r="319" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="319" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW319" s="4"/>
       <c r="AX319" s="4"/>
     </row>
-    <row r="320" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="320" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW320" s="4"/>
       <c r="AX320" s="4"/>
     </row>
-    <row r="321" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="321" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW321" s="4"/>
       <c r="AX321" s="4"/>
     </row>
-    <row r="322" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="322" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW322" s="4"/>
       <c r="AX322" s="4"/>
     </row>
-    <row r="323" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="323" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW323" s="4"/>
       <c r="AX323" s="4"/>
     </row>
-    <row r="324" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="324" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW324" s="4"/>
       <c r="AX324" s="4"/>
     </row>
-    <row r="325" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="325" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW325" s="4"/>
       <c r="AX325" s="4"/>
     </row>
-    <row r="326" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="326" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW326" s="4"/>
       <c r="AX326" s="4"/>
     </row>
-    <row r="327" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="327" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW327" s="4"/>
       <c r="AX327" s="4"/>
     </row>
-    <row r="328" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="328" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW328" s="4"/>
       <c r="AX328" s="4"/>
     </row>
-    <row r="329" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="329" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW329" s="4"/>
       <c r="AX329" s="4"/>
     </row>
-    <row r="330" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="330" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW330" s="4"/>
       <c r="AX330" s="4"/>
     </row>
-    <row r="331" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="331" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW331" s="4"/>
       <c r="AX331" s="4"/>
     </row>
-    <row r="332" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="332" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW332" s="4"/>
       <c r="AX332" s="4"/>
     </row>
-    <row r="333" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="333" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW333" s="4"/>
       <c r="AX333" s="4"/>
     </row>
-    <row r="334" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="334" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW334" s="4"/>
       <c r="AX334" s="4"/>
     </row>
-    <row r="335" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="335" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW335" s="4"/>
       <c r="AX335" s="4"/>
     </row>
-    <row r="336" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="336" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW336" s="4"/>
       <c r="AX336" s="4"/>
     </row>
-    <row r="337" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="337" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW337" s="4"/>
       <c r="AX337" s="4"/>
     </row>
-    <row r="338" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="338" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW338" s="4"/>
       <c r="AX338" s="4"/>
     </row>
-    <row r="339" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="339" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW339" s="4"/>
       <c r="AX339" s="4"/>
     </row>
-    <row r="340" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="340" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW340" s="4"/>
       <c r="AX340" s="4"/>
     </row>
-    <row r="341" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="341" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW341" s="4"/>
       <c r="AX341" s="4"/>
     </row>
-    <row r="342" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="342" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW342" s="4"/>
       <c r="AX342" s="4"/>
     </row>
-    <row r="343" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="343" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW343" s="4"/>
       <c r="AX343" s="4"/>
     </row>
-    <row r="344" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="344" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW344" s="4"/>
       <c r="AX344" s="4"/>
     </row>
-    <row r="345" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="345" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW345" s="4"/>
       <c r="AX345" s="4"/>
     </row>
-    <row r="346" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="346" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW346" s="4"/>
       <c r="AX346" s="4"/>
     </row>
-    <row r="347" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="347" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW347" s="4"/>
       <c r="AX347" s="4"/>
     </row>
-    <row r="348" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="348" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW348" s="4"/>
       <c r="AX348" s="4"/>
     </row>
-    <row r="349" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="349" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW349" s="4"/>
       <c r="AX349" s="4"/>
     </row>
-    <row r="350" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="350" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW350" s="4"/>
       <c r="AX350" s="4"/>
     </row>
-    <row r="351" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="351" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW351" s="4"/>
       <c r="AX351" s="4"/>
     </row>
-    <row r="352" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="352" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW352" s="4"/>
       <c r="AX352" s="4"/>
     </row>
-    <row r="353" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="353" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW353" s="4"/>
       <c r="AX353" s="4"/>
     </row>
-    <row r="354" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="354" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW354" s="4"/>
       <c r="AX354" s="4"/>
     </row>
-    <row r="355" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="355" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW355" s="4"/>
       <c r="AX355" s="4"/>
     </row>
-    <row r="356" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="356" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW356" s="4"/>
       <c r="AX356" s="4"/>
     </row>
-    <row r="357" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="357" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW357" s="4"/>
       <c r="AX357" s="4"/>
     </row>
-    <row r="358" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="358" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW358" s="4"/>
       <c r="AX358" s="4"/>
     </row>
-    <row r="359" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="359" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW359" s="4"/>
       <c r="AX359" s="4"/>
     </row>
-    <row r="360" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="360" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW360" s="4"/>
       <c r="AX360" s="4"/>
     </row>
-    <row r="361" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="361" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW361" s="4"/>
       <c r="AX361" s="4"/>
     </row>
-    <row r="362" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="362" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW362" s="4"/>
       <c r="AX362" s="4"/>
     </row>
-    <row r="363" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="363" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW363" s="4"/>
       <c r="AX363" s="4"/>
     </row>
-    <row r="364" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="364" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW364" s="4"/>
       <c r="AX364" s="4"/>
     </row>
-    <row r="365" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="365" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW365" s="4"/>
       <c r="AX365" s="4"/>
     </row>
-    <row r="366" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="366" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW366" s="4"/>
       <c r="AX366" s="4"/>
     </row>
-    <row r="367" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="367" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW367" s="4"/>
       <c r="AX367" s="4"/>
     </row>
-    <row r="368" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="368" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW368" s="4"/>
       <c r="AX368" s="4"/>
     </row>
-    <row r="369" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="369" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW369" s="4"/>
       <c r="AX369" s="4"/>
     </row>
-    <row r="370" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="370" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW370" s="4"/>
       <c r="AX370" s="4"/>
     </row>
-    <row r="371" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="371" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW371" s="4"/>
       <c r="AX371" s="4"/>
     </row>
-    <row r="372" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="372" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW372" s="4"/>
       <c r="AX372" s="4"/>
     </row>
-    <row r="373" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="373" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW373" s="4"/>
       <c r="AX373" s="4"/>
     </row>
-    <row r="374" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="374" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW374" s="4"/>
       <c r="AX374" s="4"/>
     </row>
-    <row r="375" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="375" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW375" s="4"/>
       <c r="AX375" s="4"/>
     </row>
-    <row r="376" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="376" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW376" s="4"/>
       <c r="AX376" s="4"/>
     </row>
-    <row r="377" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="377" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW377" s="4"/>
       <c r="AX377" s="4"/>
     </row>
-    <row r="378" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="378" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW378" s="4"/>
       <c r="AX378" s="4"/>
     </row>
-    <row r="379" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="379" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW379" s="4"/>
       <c r="AX379" s="4"/>
     </row>
-    <row r="380" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="380" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW380" s="4"/>
       <c r="AX380" s="4"/>
     </row>
-    <row r="381" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="381" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW381" s="4"/>
       <c r="AX381" s="4"/>
     </row>
-    <row r="382" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="382" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW382" s="4"/>
       <c r="AX382" s="4"/>
     </row>
-    <row r="383" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="383" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW383" s="4"/>
       <c r="AX383" s="4"/>
     </row>
-    <row r="384" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="384" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW384" s="4"/>
       <c r="AX384" s="4"/>
     </row>
-    <row r="385" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="385" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW385" s="4"/>
       <c r="AX385" s="4"/>
     </row>
-    <row r="386" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="386" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW386" s="4"/>
       <c r="AX386" s="4"/>
     </row>
-    <row r="387" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="387" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW387" s="4"/>
       <c r="AX387" s="4"/>
     </row>
-    <row r="388" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="388" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW388" s="4"/>
       <c r="AX388" s="4"/>
     </row>
-    <row r="389" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="389" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW389" s="4"/>
       <c r="AX389" s="4"/>
     </row>
-    <row r="390" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="390" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW390" s="4"/>
       <c r="AX390" s="4"/>
     </row>
-    <row r="391" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="391" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW391" s="4"/>
       <c r="AX391" s="4"/>
     </row>
-    <row r="392" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="392" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW392" s="4"/>
       <c r="AX392" s="4"/>
     </row>
-    <row r="393" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="393" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW393" s="4"/>
       <c r="AX393" s="4"/>
     </row>
-    <row r="394" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="394" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW394" s="4"/>
       <c r="AX394" s="4"/>
     </row>
-    <row r="395" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="395" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW395" s="4"/>
       <c r="AX395" s="4"/>
     </row>
-    <row r="396" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="396" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW396" s="4"/>
       <c r="AX396" s="4"/>
     </row>
-    <row r="397" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="397" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW397" s="4"/>
       <c r="AX397" s="4"/>
     </row>
-    <row r="398" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="398" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW398" s="4"/>
       <c r="AX398" s="4"/>
     </row>
-    <row r="399" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="399" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW399" s="4"/>
       <c r="AX399" s="4"/>
     </row>
-    <row r="400" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="400" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW400" s="4"/>
       <c r="AX400" s="4"/>
     </row>
-    <row r="401" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="401" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW401" s="4"/>
       <c r="AX401" s="4"/>
     </row>
-    <row r="402" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="402" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW402" s="4"/>
       <c r="AX402" s="4"/>
     </row>
-    <row r="403" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="403" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW403" s="4"/>
       <c r="AX403" s="4"/>
     </row>
-    <row r="404" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="404" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW404" s="4"/>
       <c r="AX404" s="4"/>
     </row>
-    <row r="405" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="405" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW405" s="4"/>
       <c r="AX405" s="4"/>
     </row>
-    <row r="406" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="406" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW406" s="4"/>
       <c r="AX406" s="4"/>
     </row>
-    <row r="407" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="407" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW407" s="4"/>
       <c r="AX407" s="4"/>
     </row>
-    <row r="408" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="408" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW408" s="4"/>
       <c r="AX408" s="4"/>
     </row>
-    <row r="409" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="409" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW409" s="4"/>
       <c r="AX409" s="4"/>
     </row>
-    <row r="410" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="410" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW410" s="4"/>
       <c r="AX410" s="4"/>
     </row>
-    <row r="411" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="411" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW411" s="4"/>
       <c r="AX411" s="4"/>
     </row>
-    <row r="412" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="412" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW412" s="4"/>
       <c r="AX412" s="4"/>
     </row>
-    <row r="413" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="413" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW413" s="4"/>
       <c r="AX413" s="4"/>
     </row>
-    <row r="414" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="414" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW414" s="4"/>
       <c r="AX414" s="4"/>
     </row>
-    <row r="415" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="415" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW415" s="4"/>
       <c r="AX415" s="4"/>
     </row>
-    <row r="416" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="416" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW416" s="4"/>
       <c r="AX416" s="4"/>
     </row>
-    <row r="417" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="417" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW417" s="4"/>
       <c r="AX417" s="4"/>
     </row>
-    <row r="418" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="418" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW418" s="4"/>
       <c r="AX418" s="4"/>
     </row>
-    <row r="419" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="419" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW419" s="4"/>
       <c r="AX419" s="4"/>
     </row>
-    <row r="420" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="420" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW420" s="4"/>
       <c r="AX420" s="4"/>
     </row>
-    <row r="421" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="421" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW421" s="4"/>
       <c r="AX421" s="4"/>
     </row>
-    <row r="422" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="422" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW422" s="4"/>
       <c r="AX422" s="4"/>
     </row>
-    <row r="423" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="423" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW423" s="4"/>
       <c r="AX423" s="4"/>
     </row>
-    <row r="424" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="424" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW424" s="4"/>
       <c r="AX424" s="4"/>
     </row>
-    <row r="425" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="425" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW425" s="4"/>
       <c r="AX425" s="4"/>
     </row>
-    <row r="426" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="426" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW426" s="4"/>
       <c r="AX426" s="4"/>
     </row>
-    <row r="427" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="427" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW427" s="4"/>
       <c r="AX427" s="4"/>
     </row>
-    <row r="428" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="428" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW428" s="4"/>
       <c r="AX428" s="4"/>
     </row>
-    <row r="429" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="429" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW429" s="4"/>
       <c r="AX429" s="4"/>
     </row>
-    <row r="430" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="430" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW430" s="4"/>
       <c r="AX430" s="4"/>
     </row>
-    <row r="431" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="431" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW431" s="4"/>
       <c r="AX431" s="4"/>
     </row>
-    <row r="432" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="432" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW432" s="4"/>
       <c r="AX432" s="4"/>
     </row>
-    <row r="433" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="433" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW433" s="4"/>
       <c r="AX433" s="4"/>
     </row>
-    <row r="434" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="434" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW434" s="4"/>
       <c r="AX434" s="4"/>
     </row>
-    <row r="435" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="435" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW435" s="4"/>
       <c r="AX435" s="4"/>
     </row>
-    <row r="436" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="436" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW436" s="4"/>
       <c r="AX436" s="4"/>
     </row>
-    <row r="437" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="437" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW437" s="4"/>
       <c r="AX437" s="4"/>
     </row>
-    <row r="438" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="438" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW438" s="4"/>
       <c r="AX438" s="4"/>
     </row>
-    <row r="439" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="439" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW439" s="4"/>
       <c r="AX439" s="4"/>
     </row>
-    <row r="440" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="440" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW440" s="4"/>
       <c r="AX440" s="4"/>
     </row>
-    <row r="441" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="441" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW441" s="4"/>
       <c r="AX441" s="4"/>
     </row>
-    <row r="442" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="442" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW442" s="4"/>
       <c r="AX442" s="4"/>
     </row>
-    <row r="443" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="443" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW443" s="4"/>
       <c r="AX443" s="4"/>
     </row>
-    <row r="444" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="444" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW444" s="4"/>
       <c r="AX444" s="4"/>
     </row>
-    <row r="445" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="445" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW445" s="4"/>
       <c r="AX445" s="4"/>
     </row>
-    <row r="446" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="446" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW446" s="4"/>
       <c r="AX446" s="4"/>
     </row>
-    <row r="447" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="447" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW447" s="4"/>
       <c r="AX447" s="4"/>
     </row>
-    <row r="448" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="448" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW448" s="4"/>
       <c r="AX448" s="4"/>
     </row>
-    <row r="449" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="449" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW449" s="4"/>
       <c r="AX449" s="4"/>
     </row>
-    <row r="450" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="450" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW450" s="4"/>
       <c r="AX450" s="4"/>
     </row>
-    <row r="451" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="451" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW451" s="4"/>
       <c r="AX451" s="4"/>
     </row>
-    <row r="452" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="452" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW452" s="4"/>
       <c r="AX452" s="4"/>
     </row>
-    <row r="453" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="453" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW453" s="4"/>
       <c r="AX453" s="4"/>
     </row>
-    <row r="454" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="454" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW454" s="4"/>
       <c r="AX454" s="4"/>
     </row>
-    <row r="455" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="455" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW455" s="4"/>
       <c r="AX455" s="4"/>
     </row>
-    <row r="456" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="456" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW456" s="4"/>
       <c r="AX456" s="4"/>
     </row>
-    <row r="457" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="457" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW457" s="4"/>
       <c r="AX457" s="4"/>
     </row>
-    <row r="458" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="458" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW458" s="4"/>
       <c r="AX458" s="4"/>
     </row>
-    <row r="459" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="459" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW459" s="4"/>
       <c r="AX459" s="4"/>
     </row>
-    <row r="460" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="460" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW460" s="4"/>
       <c r="AX460" s="4"/>
     </row>
-    <row r="461" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="461" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW461" s="4"/>
       <c r="AX461" s="4"/>
     </row>
-    <row r="462" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="462" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW462" s="4"/>
       <c r="AX462" s="4"/>
     </row>
-    <row r="463" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="463" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW463" s="4"/>
       <c r="AX463" s="4"/>
     </row>
-    <row r="464" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="464" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW464" s="4"/>
       <c r="AX464" s="4"/>
     </row>
-    <row r="465" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="465" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW465" s="4"/>
       <c r="AX465" s="4"/>
     </row>
-    <row r="466" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="466" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW466" s="4"/>
       <c r="AX466" s="4"/>
     </row>
-    <row r="467" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="467" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW467" s="4"/>
       <c r="AX467" s="4"/>
     </row>
-    <row r="468" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="468" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW468" s="4"/>
       <c r="AX468" s="4"/>
     </row>
-    <row r="469" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="469" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW469" s="4"/>
       <c r="AX469" s="4"/>
     </row>
-    <row r="470" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="470" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW470" s="4"/>
       <c r="AX470" s="4"/>
     </row>
-    <row r="471" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="471" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW471" s="4"/>
       <c r="AX471" s="4"/>
     </row>
-    <row r="472" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="472" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW472" s="4"/>
       <c r="AX472" s="4"/>
     </row>
-    <row r="473" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="473" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW473" s="4"/>
       <c r="AX473" s="4"/>
     </row>
-    <row r="474" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="474" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW474" s="4"/>
       <c r="AX474" s="4"/>
     </row>
-    <row r="475" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="475" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW475" s="4"/>
       <c r="AX475" s="4"/>
     </row>
-    <row r="476" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="476" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW476" s="4"/>
       <c r="AX476" s="4"/>
     </row>
-    <row r="477" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="477" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW477" s="4"/>
       <c r="AX477" s="4"/>
     </row>
-    <row r="478" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="478" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW478" s="4"/>
       <c r="AX478" s="4"/>
     </row>
-    <row r="479" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="479" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW479" s="4"/>
       <c r="AX479" s="4"/>
     </row>
-    <row r="480" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="480" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW480" s="4"/>
       <c r="AX480" s="4"/>
     </row>
-    <row r="481" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="481" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW481" s="4"/>
       <c r="AX481" s="4"/>
     </row>
-    <row r="482" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="482" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW482" s="4"/>
       <c r="AX482" s="4"/>
     </row>
-    <row r="483" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="483" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW483" s="4"/>
       <c r="AX483" s="4"/>
     </row>
-    <row r="484" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="484" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW484" s="4"/>
       <c r="AX484" s="4"/>
     </row>
-    <row r="485" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="485" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW485" s="4"/>
       <c r="AX485" s="4"/>
     </row>
-    <row r="486" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="486" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW486" s="4"/>
       <c r="AX486" s="4"/>
     </row>
-    <row r="487" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="487" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW487" s="4"/>
       <c r="AX487" s="4"/>
     </row>
-    <row r="488" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="488" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW488" s="4"/>
       <c r="AX488" s="4"/>
     </row>
-    <row r="489" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="489" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW489" s="4"/>
       <c r="AX489" s="4"/>
     </row>
-    <row r="490" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="490" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW490" s="4"/>
       <c r="AX490" s="4"/>
     </row>
-    <row r="491" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="491" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW491" s="4"/>
       <c r="AX491" s="4"/>
     </row>
-    <row r="492" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="492" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW492" s="4"/>
       <c r="AX492" s="4"/>
     </row>
-    <row r="493" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="493" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW493" s="4"/>
       <c r="AX493" s="4"/>
     </row>
-    <row r="494" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="494" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW494" s="4"/>
       <c r="AX494" s="4"/>
     </row>
-    <row r="495" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="495" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW495" s="4"/>
       <c r="AX495" s="4"/>
     </row>
-    <row r="496" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="496" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW496" s="4"/>
       <c r="AX496" s="4"/>
     </row>
-    <row r="497" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="497" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW497" s="4"/>
       <c r="AX497" s="4"/>
     </row>
-    <row r="498" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="498" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW498" s="4"/>
       <c r="AX498" s="4"/>
     </row>
-    <row r="499" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="499" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW499" s="4"/>
       <c r="AX499" s="4"/>
     </row>
-    <row r="500" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="500" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW500" s="4"/>
       <c r="AX500" s="4"/>
     </row>
-    <row r="501" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="501" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW501" s="4"/>
       <c r="AX501" s="4"/>
     </row>
-    <row r="502" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="502" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW502" s="4"/>
       <c r="AX502" s="4"/>
     </row>
-    <row r="503" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="503" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW503" s="4"/>
       <c r="AX503" s="4"/>
     </row>
-    <row r="504" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="504" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW504" s="4"/>
       <c r="AX504" s="4"/>
     </row>
-    <row r="505" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="505" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW505" s="4"/>
       <c r="AX505" s="4"/>
     </row>
-    <row r="506" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="506" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW506" s="4"/>
       <c r="AX506" s="4"/>
     </row>
-    <row r="507" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="507" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW507" s="4"/>
       <c r="AX507" s="4"/>
     </row>
-    <row r="508" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="508" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW508" s="4"/>
       <c r="AX508" s="4"/>
     </row>
-    <row r="509" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="509" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW509" s="4"/>
       <c r="AX509" s="4"/>
     </row>
-    <row r="510" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="510" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW510" s="4"/>
       <c r="AX510" s="4"/>
     </row>
-    <row r="511" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="511" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW511" s="4"/>
       <c r="AX511" s="4"/>
     </row>
-    <row r="512" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="512" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW512" s="4"/>
       <c r="AX512" s="4"/>
     </row>
-    <row r="513" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="513" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW513" s="4"/>
       <c r="AX513" s="4"/>
     </row>
-    <row r="514" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="514" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW514" s="4"/>
       <c r="AX514" s="4"/>
     </row>
-    <row r="515" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="515" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW515" s="4"/>
       <c r="AX515" s="4"/>
     </row>
-    <row r="516" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="516" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW516" s="4"/>
       <c r="AX516" s="4"/>
     </row>
-    <row r="517" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="517" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW517" s="4"/>
       <c r="AX517" s="4"/>
     </row>
-    <row r="518" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="518" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW518" s="4"/>
       <c r="AX518" s="4"/>
     </row>
-    <row r="519" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="519" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW519" s="4"/>
       <c r="AX519" s="4"/>
     </row>
-    <row r="520" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="520" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW520" s="4"/>
       <c r="AX520" s="4"/>
     </row>
-    <row r="521" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="521" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW521" s="4"/>
       <c r="AX521" s="4"/>
     </row>
-    <row r="522" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="522" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW522" s="4"/>
       <c r="AX522" s="4"/>
     </row>
-    <row r="523" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="523" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW523" s="4"/>
       <c r="AX523" s="4"/>
     </row>
-    <row r="524" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="524" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW524" s="4"/>
       <c r="AX524" s="4"/>
     </row>
-    <row r="525" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="525" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW525" s="4"/>
       <c r="AX525" s="4"/>
     </row>
-    <row r="526" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="526" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW526" s="4"/>
       <c r="AX526" s="4"/>
     </row>
-    <row r="527" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="527" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW527" s="4"/>
       <c r="AX527" s="4"/>
     </row>
-    <row r="528" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="528" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW528" s="4"/>
       <c r="AX528" s="4"/>
     </row>
-    <row r="529" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="529" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW529" s="4"/>
       <c r="AX529" s="4"/>
     </row>
-    <row r="530" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="530" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW530" s="4"/>
       <c r="AX530" s="4"/>
     </row>
-    <row r="531" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="531" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW531" s="4"/>
       <c r="AX531" s="4"/>
     </row>
-    <row r="532" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="532" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW532" s="4"/>
       <c r="AX532" s="4"/>
     </row>
-    <row r="533" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="533" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW533" s="4"/>
       <c r="AX533" s="4"/>
     </row>
-    <row r="534" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="534" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW534" s="4"/>
       <c r="AX534" s="4"/>
     </row>
-    <row r="535" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="535" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW535" s="4"/>
       <c r="AX535" s="4"/>
     </row>
-    <row r="536" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="536" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW536" s="4"/>
       <c r="AX536" s="4"/>
     </row>
-    <row r="537" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="537" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW537" s="4"/>
       <c r="AX537" s="4"/>
     </row>
-    <row r="538" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="538" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW538" s="4"/>
       <c r="AX538" s="4"/>
     </row>
-    <row r="539" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="539" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW539" s="4"/>
       <c r="AX539" s="4"/>
     </row>
-    <row r="540" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="540" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW540" s="4"/>
       <c r="AX540" s="4"/>
     </row>
-    <row r="541" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="541" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW541" s="4"/>
       <c r="AX541" s="4"/>
     </row>
-    <row r="542" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="542" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW542" s="4"/>
       <c r="AX542" s="4"/>
     </row>
-    <row r="543" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="543" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW543" s="4"/>
       <c r="AX543" s="4"/>
     </row>
-    <row r="544" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="544" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW544" s="4"/>
       <c r="AX544" s="4"/>
     </row>
-    <row r="545" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="545" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW545" s="4"/>
       <c r="AX545" s="4"/>
     </row>
-    <row r="546" spans="49:50" x14ac:dyDescent="0.25">
+    <row r="546" spans="49:50" x14ac:dyDescent="0.45">
       <c r="AW546" s="4"/>
       <c r="AX546" s="4"/>
     </row>

</xml_diff>